<commit_message>
Update borehole and sounding purpose codelists
</commit_message>
<xml_diff>
--- a/Draft Excel Codelists/boreholePurpose.xlsx
+++ b/Draft Excel Codelists/boreholePurpose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lpeve\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Draft Excel Codelists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8322FD1-F01B-4955-8725-2A51AACBDE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0F28CF-3F87-374F-9CC8-5591B294A596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51220" windowHeight="27180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="379">
   <si>
     <t>Description</t>
   </si>
@@ -746,12 +746,6 @@
     <t>boreholePurpose</t>
   </si>
   <si>
-    <t>DIGGS Borehole Purpose</t>
-  </si>
-  <si>
-    <t>A description of the purpose for drilling the hole (eg. exploratory boring, monitoring well, etc.)</t>
-  </si>
-  <si>
     <t>IB</t>
   </si>
   <si>
@@ -1122,6 +1116,66 @@
   </si>
   <si>
     <t>SES</t>
+  </si>
+  <si>
+    <t>DIGGS Borehole Purpose Codelist Definitions</t>
+  </si>
+  <si>
+    <t>Codes that define the purpose of a borehole. These codes are used for the value of the boreholePurpose property of the Borehole object.)</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>Crosshole Seismic Test</t>
+  </si>
+  <si>
+    <t>DST</t>
+  </si>
+  <si>
+    <t>Downhole Seismic Test</t>
+  </si>
+  <si>
+    <t>IVAN</t>
+  </si>
+  <si>
+    <t>INST</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>PET</t>
+  </si>
+  <si>
+    <t>PLT</t>
+  </si>
+  <si>
+    <t>PMT</t>
+  </si>
+  <si>
+    <t>SPT</t>
+  </si>
+  <si>
+    <t>Insitu Vane Shear</t>
+  </si>
+  <si>
+    <t>instrument</t>
+  </si>
+  <si>
+    <t>Monitoring Well</t>
+  </si>
+  <si>
+    <t>Permeability Test</t>
+  </si>
+  <si>
+    <t>Plate Load Test</t>
+  </si>
+  <si>
+    <t>Pressuremeter</t>
+  </si>
+  <si>
+    <t>Standard Penetration Test</t>
   </si>
 </sst>
 </file>
@@ -1230,6 +1284,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1339,6 +1394,59 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1406,59 +1514,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1533,39 +1588,36 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H42" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H42" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H1">
-    <sortCondition ref="C1"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H51" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:H51" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="11">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2790,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D68" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D68" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:D68" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
     <sortCondition ref="B1:B68"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="12">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="2">
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1853,20 +1905,20 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="A12:E13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="41.375" customWidth="1"/>
-    <col min="3" max="3" width="26.375" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="76" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1883,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1892,7 +1944,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>234</v>
       </c>
@@ -1900,10 +1952,10 @@
         <v>234</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>235</v>
+        <v>359</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>236</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -1918,26 +1970,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="84.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="84.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1963,812 +2015,983 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2810,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2810,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="C8" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B2821,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2822,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2820,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2810,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2810,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="E19" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2821,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2822,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2824,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D22" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="E22" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2825,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+      <c r="C23" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2826,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B2821,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>337</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>321</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2822,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B17" s="13" t="s">
+      <c r="C24" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2828,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2829,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2830,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2831,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2832,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2832,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2833,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2834,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B2835,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B2836,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B2837,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B2838,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B2839,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2820,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2821,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2822,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2824,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2825,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B23" s="13" t="s">
+      <c r="C37" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B2840,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B2841,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B41,AssociatedElements!B$2:B2843,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2826,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2828,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2829,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2830,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2831,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B28" s="13" t="s">
+      <c r="C41" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B42,AssociatedElements!B$2:B2844,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B42" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2832,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>318</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2832,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2833,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2834,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B2835,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B2836,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B2837,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B2838,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B2839,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B2840,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B2841,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B41,AssociatedElements!B$2:B2843,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="C41" s="13" t="s">
+      <c r="C42" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D42" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="E41" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B42,AssociatedElements!B$2:B2844,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>316</v>
-      </c>
       <c r="E42" s="14" t="s">
         <v>4</v>
       </c>
       <c r="G42" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B43,AssociatedElements!B$2:B2831,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D43" s="13"/>
+      <c r="E43" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B44,AssociatedElements!B$2:B2832,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="D44" s="13"/>
+      <c r="E44" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B45,AssociatedElements!B$2:B2833,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B46,AssociatedElements!B$2:B2834,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="D46" s="13"/>
+      <c r="E46" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B47,AssociatedElements!B$2:B2835,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D47" s="13"/>
+      <c r="E47" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B48,AssociatedElements!B$2:B2836,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="D48" s="13"/>
+      <c r="E48" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B49,AssociatedElements!B$2:B2838,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B50,AssociatedElements!B$2:B2839,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B51,AssociatedElements!B$2:B2840,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="14" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2786,13 +3009,13 @@
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$178</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F42</xm:sqref>
+          <xm:sqref>F2:F51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
-            <xm:f>'C:\Users\dponti\GitHub\diggs-dictionaries\[DIGGSDictionaryClassificationCodeASTMD2487.xlsx]Lists'!#REF!</xm:f>
+            <xm:f>'/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/C:\Users\dponti\GitHub\diggs-dictionaries\[DIGGSDictionaryClassificationCodeASTMD2487.xlsx]Lists'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E42</xm:sqref>
+          <xm:sqref>E2:E51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2807,18 +3030,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="A1:D14"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.125" customWidth="1"/>
-    <col min="2" max="2" width="31.625" customWidth="1"/>
-    <col min="3" max="3" width="86.125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="86.1640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="93" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -2832,474 +3055,519 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B2" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="C8" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="C10" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="C11" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="C13" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B12" s="15" t="s">
+      <c r="C15" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1692,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B14" s="13" t="s">
+      <c r="C23" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1693,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="C24" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+      <c r="C37" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B38" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B39" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B41" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
+      <c r="C41" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B42" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
-        <v>353</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="15" t="s">
-        <v>354</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="15" t="s">
-        <v>352</v>
-      </c>
       <c r="C42" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="13"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="15"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="15"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="15"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="15"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="15"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="13"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="15"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="15"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B43" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B45" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B46" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B47" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B48" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B49" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B50" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B51" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" s="13"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" s="13"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" s="13"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" s="15"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" s="15"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B63" s="13"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B64" s="13"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="13"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" s="15"/>
     </row>
   </sheetData>
@@ -3323,13 +3591,13 @@
       <selection activeCell="A2" sqref="A2:A187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.125" customWidth="1"/>
-    <col min="3" max="3" width="54.125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="54.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -3340,7 +3608,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>179</v>
       </c>
@@ -3349,7 +3617,7 @@
       </c>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>175</v>
       </c>
@@ -3358,7 +3626,7 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>174</v>
       </c>
@@ -3367,7 +3635,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
         <v>189</v>
       </c>
@@ -3376,7 +3644,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>168</v>
       </c>
@@ -3385,7 +3653,7 @@
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>167</v>
       </c>
@@ -3394,7 +3662,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>178</v>
       </c>
@@ -3403,7 +3671,7 @@
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
         <v>1</v>
       </c>
@@ -3412,7 +3680,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>166</v>
       </c>
@@ -3421,7 +3689,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>177</v>
       </c>
@@ -3430,7 +3698,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>172</v>
       </c>
@@ -3439,7 +3707,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>173</v>
       </c>
@@ -3448,7 +3716,7 @@
       </c>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>171</v>
       </c>
@@ -3457,7 +3725,7 @@
       </c>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>170</v>
       </c>
@@ -3466,7 +3734,7 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>169</v>
       </c>
@@ -3475,7 +3743,7 @@
       </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>176</v>
       </c>
@@ -3484,14 +3752,14 @@
       </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
       <c r="C18" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>180</v>
       </c>
@@ -3500,7 +3768,7 @@
       </c>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>232</v>
       </c>
@@ -3509,7 +3777,7 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
         <v>182</v>
       </c>
@@ -3518,7 +3786,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>184</v>
       </c>
@@ -3527,7 +3795,7 @@
       </c>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>183</v>
       </c>
@@ -3536,7 +3804,7 @@
       </c>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>181</v>
       </c>
@@ -3545,7 +3813,7 @@
       </c>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>192</v>
       </c>
@@ -3554,7 +3822,7 @@
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>186</v>
       </c>
@@ -3563,7 +3831,7 @@
       </c>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>187</v>
       </c>
@@ -3572,7 +3840,7 @@
       </c>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="11" t="s">
         <v>4</v>
       </c>
@@ -3581,13 +3849,13 @@
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>25</v>
       </c>
@@ -3596,7 +3864,7 @@
       </c>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>193</v>
       </c>
@@ -3605,7 +3873,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>191</v>
       </c>
@@ -3614,7 +3882,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>188</v>
       </c>
@@ -3623,7 +3891,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>185</v>
       </c>
@@ -3632,7 +3900,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>190</v>
       </c>
@@ -3641,7 +3909,7 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
         <v>231</v>
       </c>
@@ -3650,907 +3918,907 @@
       </c>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>50</v>
       </c>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>51</v>
       </c>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>52</v>
       </c>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>53</v>
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>54</v>
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>55</v>
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>56</v>
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>24</v>
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>57</v>
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
         <v>58</v>
       </c>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
         <v>59</v>
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>60</v>
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
         <v>61</v>
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
         <v>62</v>
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
         <v>63</v>
       </c>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
         <v>64</v>
       </c>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
         <v>65</v>
       </c>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
         <v>203</v>
       </c>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
         <v>66</v>
       </c>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
         <v>67</v>
       </c>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
         <v>68</v>
       </c>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>18</v>
       </c>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
         <v>69</v>
       </c>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
         <v>70</v>
       </c>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>71</v>
       </c>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>72</v>
       </c>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>73</v>
       </c>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
         <v>74</v>
       </c>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>75</v>
       </c>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
         <v>76</v>
       </c>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
         <v>77</v>
       </c>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
         <v>78</v>
       </c>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
         <v>2</v>
       </c>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>19</v>
       </c>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>79</v>
       </c>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
         <v>80</v>
       </c>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
         <v>81</v>
       </c>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
         <v>23</v>
       </c>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
         <v>82</v>
       </c>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>83</v>
       </c>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
         <v>84</v>
       </c>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
         <v>85</v>
       </c>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
         <v>86</v>
       </c>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>87</v>
       </c>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
         <v>88</v>
       </c>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
         <v>89</v>
       </c>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
         <v>90</v>
       </c>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
         <v>91</v>
       </c>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
         <v>92</v>
       </c>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
         <v>93</v>
       </c>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
         <v>94</v>
       </c>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
         <v>95</v>
       </c>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
         <v>96</v>
       </c>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
         <v>97</v>
       </c>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
         <v>98</v>
       </c>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
         <v>99</v>
       </c>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
         <v>100</v>
       </c>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C98" t="s">
         <v>101</v>
       </c>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>102</v>
       </c>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C100" t="s">
         <v>103</v>
       </c>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
         <v>104</v>
       </c>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
         <v>105</v>
       </c>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
         <v>204</v>
       </c>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
         <v>205</v>
       </c>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
         <v>17</v>
       </c>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C106" t="s">
         <v>206</v>
       </c>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
         <v>207</v>
       </c>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
         <v>208</v>
       </c>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C109" t="s">
         <v>106</v>
       </c>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C110" t="s">
         <v>107</v>
       </c>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
         <v>108</v>
       </c>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C112" t="s">
         <v>109</v>
       </c>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
         <v>110</v>
       </c>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C114" t="s">
         <v>111</v>
       </c>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
         <v>112</v>
       </c>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
         <v>113</v>
       </c>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C117" t="s">
         <v>114</v>
       </c>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C118" t="s">
         <v>115</v>
       </c>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
         <v>116</v>
       </c>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C120" t="s">
         <v>117</v>
       </c>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
         <v>11</v>
       </c>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
         <v>118</v>
       </c>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C123" t="s">
         <v>119</v>
       </c>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C124" t="s">
         <v>120</v>
       </c>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C125" t="s">
         <v>121</v>
       </c>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C126" t="s">
         <v>122</v>
       </c>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C127" t="s">
         <v>3</v>
       </c>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C128" t="s">
         <v>197</v>
       </c>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C129" t="s">
         <v>123</v>
       </c>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C130" t="s">
         <v>124</v>
       </c>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C131" t="s">
         <v>125</v>
       </c>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C132" t="s">
         <v>209</v>
       </c>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C133" t="s">
         <v>126</v>
       </c>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C134" t="s">
         <v>127</v>
       </c>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C135" t="s">
         <v>128</v>
       </c>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C136" t="s">
         <v>129</v>
       </c>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C137" t="s">
         <v>130</v>
       </c>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C138" t="s">
         <v>131</v>
       </c>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C139" t="s">
         <v>132</v>
       </c>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C140" t="s">
         <v>133</v>
       </c>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C141" t="s">
         <v>134</v>
       </c>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C142" t="s">
         <v>210</v>
       </c>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C143" t="s">
         <v>135</v>
       </c>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C144" t="s">
         <v>136</v>
       </c>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C145" t="s">
         <v>222</v>
       </c>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C146" t="s">
         <v>137</v>
       </c>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C147" t="s">
         <v>138</v>
       </c>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
         <v>139</v>
       </c>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
         <v>140</v>
       </c>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C150" t="s">
         <v>141</v>
       </c>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C151" t="s">
         <v>142</v>
       </c>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
         <v>143</v>
       </c>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
         <v>144</v>
       </c>
       <c r="D153" s="8"/>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C154" t="s">
         <v>145</v>
       </c>
       <c r="D154" s="8"/>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C155" t="s">
         <v>146</v>
       </c>
       <c r="D155" s="8"/>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
         <v>147</v>
       </c>
       <c r="D156" s="8"/>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C157" t="s">
         <v>148</v>
       </c>
       <c r="D157" s="8"/>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C158" t="s">
         <v>149</v>
       </c>
       <c r="D158" s="8"/>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C159" t="s">
         <v>150</v>
       </c>
       <c r="D159" s="8"/>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C160" t="s">
         <v>151</v>
       </c>
       <c r="D160" s="8"/>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C161" t="s">
         <v>22</v>
       </c>
       <c r="D161" s="8"/>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C162" t="s">
         <v>211</v>
       </c>
       <c r="D162" s="8"/>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C163" t="s">
         <v>25</v>
       </c>
       <c r="D163" s="8"/>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C164" t="s">
         <v>21</v>
       </c>
       <c r="D164" s="8"/>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C165" t="s">
         <v>152</v>
       </c>
       <c r="D165" s="8"/>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C166" t="s">
         <v>153</v>
       </c>
       <c r="D166" s="8"/>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C167" t="s">
         <v>154</v>
       </c>
       <c r="D167" s="8"/>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C168" t="s">
         <v>220</v>
       </c>
       <c r="D168" s="8"/>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C169" t="s">
         <v>212</v>
       </c>
       <c r="D169" s="8"/>
     </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C170" t="s">
         <v>155</v>
       </c>
       <c r="D170" s="8"/>
     </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C171" t="s">
         <v>156</v>
       </c>
       <c r="D171" s="8"/>
     </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C172" t="s">
         <v>157</v>
       </c>
       <c r="D172" s="8"/>
     </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C173" t="s">
         <v>158</v>
       </c>
       <c r="D173" s="8"/>
     </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C174" t="s">
         <v>159</v>
       </c>
       <c r="D174" s="8"/>
     </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C175" t="s">
         <v>160</v>
       </c>
       <c r="D175" s="8"/>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C176" t="s">
         <v>161</v>
       </c>
       <c r="D176" s="8"/>
     </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C177" t="s">
         <v>162</v>
       </c>
       <c r="D177" s="8"/>
     </row>
-    <row r="178" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C178" t="s">
         <v>213</v>
       </c>
       <c r="D178" s="8"/>
     </row>
-    <row r="179" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C179" t="s">
         <v>214</v>
       </c>
       <c r="D179" s="8"/>
     </row>
-    <row r="180" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C180" t="s">
         <v>215</v>
       </c>
       <c r="D180" s="8"/>
     </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C181" t="s">
         <v>216</v>
       </c>
       <c r="D181" s="8"/>
     </row>
-    <row r="182" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C182" t="s">
         <v>217</v>
       </c>
       <c r="D182" s="8"/>
     </row>
-    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C183" t="s">
         <v>218</v>
       </c>
       <c r="D183" s="8"/>
     </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C184" t="s">
         <v>219</v>
       </c>
       <c r="D184" s="8"/>
     </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C185" t="s">
         <v>12</v>
       </c>
       <c r="D185" s="8"/>
     </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C186" t="s">
         <v>163</v>
       </c>
       <c r="D186" s="9"/>
     </row>
-    <row r="187" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C187" t="s">
         <v>164</v>
       </c>

</xml_diff>